<commit_message>
changes to add new players
</commit_message>
<xml_diff>
--- a/data/player_stats.xlsx
+++ b/data/player_stats.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="30">
   <si>
     <t>Player</t>
   </si>
@@ -44,25 +44,79 @@
     <t>Wickets</t>
   </si>
   <si>
+    <t>QuantumQuirk</t>
+  </si>
+  <si>
+    <t>T20</t>
+  </si>
+  <si>
+    <t>ODI</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>CodeCricketMaster</t>
+  </si>
+  <si>
+    <t>RunMachine</t>
+  </si>
+  <si>
+    <t>Ava</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Ved</t>
+  </si>
+  <si>
+    <t>Sricharan</t>
+  </si>
+  <si>
+    <t>db1_db2</t>
+  </si>
+  <si>
+    <t>ady_chak</t>
+  </si>
+  <si>
+    <t>Angel</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>sammat</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>Prateesh</t>
+  </si>
+  <si>
+    <t>Bawandar</t>
+  </si>
+  <si>
+    <t>GentleGamer</t>
+  </si>
+  <si>
+    <t>Crabby</t>
+  </si>
+  <si>
+    <t>GeniiExE</t>
+  </si>
+  <si>
+    <t>Dosu</t>
+  </si>
+  <si>
+    <t>newGuy</t>
+  </si>
+  <si>
+    <t>Maverick</t>
+  </si>
+  <si>
     <t>AnkitGamer</t>
-  </si>
-  <si>
-    <t>T20</t>
-  </si>
-  <si>
-    <t>ODI</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Maverick</t>
-  </si>
-  <si>
-    <t>newGuy</t>
-  </si>
-  <si>
-    <t>rabjot_singh</t>
   </si>
 </sst>
 </file>
@@ -75,7 +129,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,13 +139,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -561,148 +608,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1057,15 +1104,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.4444444444444" customWidth="1"/>
+    <col min="1" max="1" width="18.2222222222222" customWidth="1"/>
     <col min="2" max="2" width="7.66666666666667" customWidth="1"/>
     <col min="3" max="3" width="8.88888888888889" customWidth="1"/>
     <col min="4" max="4" width="5.77777777777778" customWidth="1"/>
@@ -1293,6 +1340,924 @@
         <v>0</v>
       </c>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>23</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" t="s">
+        <v>7</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>24</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>26</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>28</v>
+      </c>
+      <c r="B64" t="s">
+        <v>8</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>29</v>
+      </c>
+      <c r="B65" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>29</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>29</v>
+      </c>
+      <c r="B67" t="s">
+        <v>8</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>